<commit_message>
result an disc TEM geschreven
</commit_message>
<xml_diff>
--- a/Measurement_Results/TEM/0.8.xlsx
+++ b/Measurement_Results/TEM/0.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="28720" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <dimension ref="A1:L458"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="40" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,20 +503,20 @@
         <v>4</v>
       </c>
       <c r="E5" s="2">
-        <f>AVERAGE(A46:A458)</f>
-        <v>49.425617433414068</v>
+        <f>AVERAGE(A2:A458)</f>
+        <v>46.746553610503327</v>
       </c>
       <c r="F5" s="2">
-        <f>STDEV(A46:A458)</f>
-        <v>5.3618623506994911</v>
+        <f>STDEV(A2:A458)</f>
+        <v>9.9720486487005342</v>
       </c>
       <c r="G5" s="2">
         <f>F5/SQRT(H5)</f>
-        <v>0.26383999786652867</v>
+        <v>0.46647276065998378</v>
       </c>
       <c r="H5" s="2">
-        <f>COUNT(A46:A458)</f>
-        <v>413</v>
+        <f>COUNT(A2:A458)</f>
+        <v>457</v>
       </c>
       <c r="L5" s="2"/>
     </row>

</xml_diff>